<commit_message>
Added FaultInjectionLidar lines for setting rain
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfigExpBmap1goal1.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfigExpBmap1goal1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C774D65C-BF91-4AFB-BC16-C6035069EB04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16092" yWindow="2712" windowWidth="14736" windowHeight="10200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16095" yWindow="2715" windowWidth="14730" windowHeight="10200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>BlockName</t>
   </si>
@@ -88,12 +87,24 @@
   </si>
   <si>
     <t>fi_lidar_rain_intensity</t>
+  </si>
+  <si>
+    <t>FaultInjectionLidar1</t>
+  </si>
+  <si>
+    <t>FaultInjectionLidar2</t>
+  </si>
+  <si>
+    <t>FaultInjectionLidar3</t>
+  </si>
+  <si>
+    <t>FaultInjectionLidar4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,19 +449,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -466,7 +477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -474,7 +485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -482,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -490,7 +501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -498,7 +509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -506,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -514,7 +525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -522,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -530,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -538,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -546,7 +557,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -554,7 +565,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -562,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -570,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -578,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -586,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -594,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -602,11 +613,43 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
         <v>0</v>
       </c>
     </row>

</xml_diff>